<commit_message>
finished merge part, also added a bunch of bed coverage calc funcs
Former-commit-id: a953b428f42bda2bd9453ad5238a2dcaaa9568e5 [formerly 674e1a1e98c627510c5f22a08bf128319b621f04]
Former-commit-id: 9b89bd5a352397cb1915d140434dd48965609a1c
</commit_message>
<xml_diff>
--- a/tests/data/sampleinfo.xlsx
+++ b/tests/data/sampleinfo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="460" windowWidth="26960" windowHeight="15380" tabRatio="500"/>
+    <workbookView xWindow="4460" yWindow="2820" windowWidth="26960" windowHeight="15380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H3" sqref="H3:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,8 +472,8 @@
         <v>Fev_DR_m70_1623.chr1.bw</v>
       </c>
       <c r="H2" t="str">
-        <f>CONCATENATE(B2,".sj.bed.gz")</f>
-        <v>Fev_DR_m70_1623.sj.bed.gz</v>
+        <f>CONCATENATE(B2,".chr1.sj.bed.gz")</f>
+        <v>Fev_DR_m70_1623.chr1.sj.bed.gz</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -502,8 +502,8 @@
         <v>Fev_CSm_m70_1624.chr1.bw</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H5" si="3">CONCATENATE(B3,".sj.bed.gz")</f>
-        <v>Fev_CSm_m70_1624.sj.bed.gz</v>
+        <f t="shared" ref="H3:H5" si="3">CONCATENATE(B3,".chr1.sj.bed.gz")</f>
+        <v>Fev_CSm_m70_1624.chr1.sj.bed.gz</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -533,7 +533,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="3"/>
-        <v>Fev_DR_m71_1625.sj.bed.gz</v>
+        <v>Fev_DR_m71_1625.chr1.sj.bed.gz</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" si="3"/>
-        <v>Fev_CSm_m71_1626.sj.bed.gz</v>
+        <v>Fev_CSm_m71_1626.chr1.sj.bed.gz</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change normalization to NONE, fix tests
Former-commit-id: 4204d9c84a2af6d3c4161c9a77da69442942d319 [formerly 0f9baab1c8dfd1d62bab9263c8a2ab85db2338c5]
Former-commit-id: 3a52a7e3bece07047c043f36ac96e60f8ce3b6cb
</commit_message>
<xml_diff>
--- a/tests/data/sampleinfo.xlsx
+++ b/tests/data/sampleinfo.xlsx
@@ -426,17 +426,17 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="7" max="7" width="34.33203125" customWidth="1"/>
+    <col min="7" max="7" width="38.33203125" customWidth="1"/>
     <col min="8" max="8" width="31.6640625" customWidth="1"/>
     <col min="9" max="9" width="27.83203125" customWidth="1"/>
     <col min="10" max="10" width="33.1640625" customWidth="1"/>
@@ -494,8 +494,8 @@
         <v>1623.chr1</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B5" si="1">CONCATENATE(E2,".",C2)</f>
-        <v>Fev_DR_m70_1623.chr1</v>
+        <f>CONCATENATE(E2,".",C2,".17mb")</f>
+        <v>Fev_DR_m70_1623.chr1.17mb</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -510,19 +510,19 @@
         <v>10</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G5" si="2">CONCATENATE(E2,"_star.",C2,".bed.gz")</f>
-        <v>Fev_DR_m70_1623_star.chr1.bed.gz</v>
+        <f>CONCATENATE(E2,"_star.",C2,".17mb.bed.gz")</f>
+        <v>Fev_DR_m70_1623_star.chr1.17mb.bed.gz</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H5" si="3">CONCATENATE( E2, ".",C2,".SJ.out.tab")</f>
+        <f t="shared" ref="H2:H5" si="1">CONCATENATE( E2, ".",C2,".SJ.out.tab")</f>
         <v>Fev_DR_m70_1623.chr1.SJ.out.tab</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I5" si="4">CONCATENATE(E2, ".",C2,".bw")</f>
+        <f t="shared" ref="I2:I5" si="2">CONCATENATE(E2, ".",C2,".bw")</f>
         <v>Fev_DR_m70_1623.chr1.bw</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J5" si="5">CONCATENATE(E2,".",C2,".sj.bed.gz")</f>
+        <f t="shared" ref="J2:J5" si="3">CONCATENATE(E2,".",C2,".sj.bed.gz")</f>
         <v>Fev_DR_m70_1623.chr1.sj.bed.gz</v>
       </c>
       <c r="K2">
@@ -544,8 +544,8 @@
         <v>1624.chr1</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" si="1"/>
-        <v>Fev_CSm_m70_1624.chr1</v>
+        <f t="shared" ref="B3:B5" si="4">CONCATENATE(E3,".",C3,".17mb")</f>
+        <v>Fev_CSm_m70_1624.chr1.17mb</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -560,19 +560,19 @@
         <v>8</v>
       </c>
       <c r="G3" t="str">
+        <f t="shared" ref="G3:G5" si="5">CONCATENATE(E3,"_star.",C3,".17mb.bed.gz")</f>
+        <v>Fev_CSm_m70_1624_star.chr1.17mb.bed.gz</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="1"/>
+        <v>Fev_CSm_m70_1624.chr1.SJ.out.tab</v>
+      </c>
+      <c r="I3" t="str">
         <f t="shared" si="2"/>
-        <v>Fev_CSm_m70_1624_star.chr1.bed.gz</v>
-      </c>
-      <c r="H3" t="str">
+        <v>Fev_CSm_m70_1624.chr1.bw</v>
+      </c>
+      <c r="J3" t="str">
         <f t="shared" si="3"/>
-        <v>Fev_CSm_m70_1624.chr1.SJ.out.tab</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" si="4"/>
-        <v>Fev_CSm_m70_1624.chr1.bw</v>
-      </c>
-      <c r="J3" t="str">
-        <f t="shared" si="5"/>
         <v>Fev_CSm_m70_1624.chr1.sj.bed.gz</v>
       </c>
       <c r="K3">
@@ -594,8 +594,8 @@
         <v>1625.chr1</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="1"/>
-        <v>Fev_DR_m71_1625.chr1</v>
+        <f t="shared" si="4"/>
+        <v>Fev_DR_m71_1625.chr1.17mb</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -610,19 +610,19 @@
         <v>10</v>
       </c>
       <c r="G4" t="str">
+        <f t="shared" si="5"/>
+        <v>Fev_DR_m71_1625_star.chr1.17mb.bed.gz</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fev_DR_m71_1625.chr1.SJ.out.tab</v>
+      </c>
+      <c r="I4" t="str">
         <f t="shared" si="2"/>
-        <v>Fev_DR_m71_1625_star.chr1.bed.gz</v>
-      </c>
-      <c r="H4" t="str">
+        <v>Fev_DR_m71_1625.chr1.bw</v>
+      </c>
+      <c r="J4" t="str">
         <f t="shared" si="3"/>
-        <v>Fev_DR_m71_1625.chr1.SJ.out.tab</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="4"/>
-        <v>Fev_DR_m71_1625.chr1.bw</v>
-      </c>
-      <c r="J4" t="str">
-        <f t="shared" si="5"/>
         <v>Fev_DR_m71_1625.chr1.sj.bed.gz</v>
       </c>
       <c r="K4">
@@ -644,8 +644,8 @@
         <v>1626.chr1</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="1"/>
-        <v>Fev_CSm_m71_1626.chr1</v>
+        <f t="shared" si="4"/>
+        <v>Fev_CSm_m71_1626.chr1.17mb</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -660,19 +660,19 @@
         <v>8</v>
       </c>
       <c r="G5" t="str">
+        <f t="shared" si="5"/>
+        <v>Fev_CSm_m71_1626_star.chr1.17mb.bed.gz</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>Fev_CSm_m71_1626.chr1.SJ.out.tab</v>
+      </c>
+      <c r="I5" t="str">
         <f t="shared" si="2"/>
-        <v>Fev_CSm_m71_1626_star.chr1.bed.gz</v>
-      </c>
-      <c r="H5" t="str">
+        <v>Fev_CSm_m71_1626.chr1.bw</v>
+      </c>
+      <c r="J5" t="str">
         <f t="shared" si="3"/>
-        <v>Fev_CSm_m71_1626.chr1.SJ.out.tab</v>
-      </c>
-      <c r="I5" t="str">
-        <f t="shared" si="4"/>
-        <v>Fev_CSm_m71_1626.chr1.bw</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" si="5"/>
         <v>Fev_CSm_m71_1626.chr1.sj.bed.gz</v>
       </c>
       <c r="K5">
@@ -729,5 +729,6 @@
     <sortCondition ref="D2:D5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>